<commit_message>
Implementa o recurso de gerar relatórios para processos de Tomada de Preço
</commit_message>
<xml_diff>
--- a/relacao_contratos.xlsx
+++ b/relacao_contratos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Registro de preços para futura e eventual aquisição de mobiliários diversos para equipar as unidades de saúde deste município</t>
   </si>
@@ -39,6 +39,45 @@
   </si>
   <si>
     <t>175/2023</t>
+  </si>
+  <si>
+    <t>Registro de preço para futura e eventual contratação de empresa especializada na realização de exames patológicos junto a Secretaria de Saúde deste município</t>
+  </si>
+  <si>
+    <t>147/2023</t>
+  </si>
+  <si>
+    <t>063/2023</t>
+  </si>
+  <si>
+    <t>Contratação de empresa com profissional médico na área de ortopedia, destinado à prestação de serviços junto a Secretaria Municipal de Saúde e Fundação Coronel João de Almeida, neste município</t>
+  </si>
+  <si>
+    <t>190/2023</t>
+  </si>
+  <si>
+    <t>081/2023</t>
+  </si>
+  <si>
+    <t>contratação de empresa com profissional cirurgião dentista para prestar serviços em unidades básicas de saúde</t>
+  </si>
+  <si>
+    <t>161/2023</t>
+  </si>
+  <si>
+    <t>069/2023</t>
+  </si>
+  <si>
+    <t>Contratação de empresa com profissional médico especializado na área de cardiologia, para realização de consultas em unidade de saúde deste município e realização de procedimentos em consultório clínico da contratada</t>
+  </si>
+  <si>
+    <t>139/2023</t>
+  </si>
+  <si>
+    <t>061/2023</t>
+  </si>
+  <si>
+    <t>15/08/2023</t>
   </si>
 </sst>
 </file>
@@ -74,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,6 +428,74 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45159</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45230</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45184</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>45167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>